<commit_message>
Screenshot/Capture file name updates
</commit_message>
<xml_diff>
--- a/AOS-GUI/AOS-GUI-OrderEntry-Laptop/Default.xlsx
+++ b/AOS-GUI/AOS-GUI-OrderEntry-Laptop/Default.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>Browser</t>
   </si>
@@ -23,13 +23,7 @@
     <t>device_manufacturer</t>
   </si>
   <si>
-    <t>CHROME</t>
-  </si>
-  <si>
     <t>device_model</t>
-  </si>
-  <si>
-    <t>FIREFOX64</t>
   </si>
   <si>
     <t>device_ostype</t>
@@ -182,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -190,43 +184,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -525,19 +489,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.71875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.63671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.9375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1484375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.41796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.95703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row ht="12.75" customHeight="1" customFormat="1">
@@ -545,30 +509,14 @@
         <v>0</v>
       </c>
       <c t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c t="s">
         <v>1</v>
       </c>
       <c t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>4</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>2</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="3"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -590,7 +538,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="16384" width="9.1484375" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row ht="12.75" customHeight="1" customFormat="1"/>

</xml_diff>